<commit_message>
Fixed error in headers collected from trustpilot reviews
</commit_message>
<xml_diff>
--- a/trustpilot_reviews/trustpilot_reviews/trustpilot.xlsx
+++ b/trustpilot_reviews/trustpilot_reviews/trustpilot.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>If you are in need of an hones tGarage look no further.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -503,76 +503,76 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Really impressed!</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Booked my car in for the second year for a major service and MOT this time.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Not what I asked for</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Booked my car in for the second year for a major service and MOT this time.</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>If you are in need of an hones tGarage look no further.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Centralautopoint</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>If you are in need of an honest reliable and friendly garage you found it.</t>
+          <t>my favorite website they are proven to pay me now I just work at home in this time of pandemic now they really pay thank you</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>AMAZING</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>I was not disappointed.</t>
+          <t>Outstanding application to feel free from threats. Enjoy to use twitter more than before with this friendly app...</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Not what I asked for</t>
+          <t>comfertbility</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Booked my car in for the second year for a major service and MOT this time.</t>
+          <t>Very good service for the affordable price! Their IPTV activation is very fast and customer support also best. It’s the best streaming service with full HD quality. My experience is great on bestiptvfrance. Highly recommended service!!!</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>If you are in need of an hones tGarage look no further.</t>
+          <t>Very good service for the affordable…</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>E.ON SE</t>
+          <t>Facebook</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The wait on phone is really bad 1 half hours disgraceful.</t>
+          <t>So I joined facebook about 2 months ago and literally the only thing I did was join my town's community page. I didn't post anything I didn't add anyone I didn't write any comments and in fact I haven't even gone on the platform in quite some time. Despite all this my account has been disabled FOUR TIMES for supposedly "violating the community standards". And somehow I've been on instagram for nearly a year and NEVER ONCE had this problem. Honestly as soon as it gets re-enabled again I'm just deleting my account because I'm sick of dealing with this</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>artificial picture of lives</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -582,568 +582,568 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Looks like the only was is to cancel my direct debit to get them to contact me they will try and charge me for it but I've done everything possible so good luck with that.</t>
+          <t>THANK YOU VERY VERY MUCH FOR BEING IMPECCABLY FLAWLESS AND IMMACULATE TO THE VERY HIGHEST DEGREE!</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Can't get hold of eon customer service</t>
+          <t>ABSOLUTE PERFECTION GUARANTEED</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Can't get hold of eon customer service phoned them and was on hold for an hour with no answer went on the online chat and was told to phone them tried to send them an email and it was returned went on FB messenger and was told to wait.</t>
+          <t xml:space="preserve">ABSOLUTE PERFECTION GUARANTEED! It successfully taught me the importance of responsible communication! I became a lot more diplomatic tactful courteous and respectful! </t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>The wait on phone is really bad 1 half…</t>
+          <t>Worst service I've ever gotten from a website</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mr Clutch</t>
+          <t>etyres</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fodi in Leyton branch best man very helpfulservice was great highly recommend !</t>
+          <t>Great service ordered my tyres paid extra for mobile tyre fitter. Tyres came with fitter and the guy fitted them within 20 minutes.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Fantastic tyre service</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Warning! We’ve detected misuse on this page</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">I booked my car in at the Chelmsford branch and Chris was my first contact a delightful man with perfect manners and so helpful I limped my car into the Chelmsford branch and as he promised Chris and his team had my car running perfectly by mid day I am very satisfied and will be using them for any job that comes up in the future. </t>
+          <t>Abysmal!!!</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Excellent service from the manager…</t>
+          <t>Abysmal!!!</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Excellent service from the manager Steve I really cannot recommend them enough. Got my MOT done at the Chingford branch! Well done guys i appreciate it!</t>
+          <t>Brilliant easy to navigate website and cheapest tyres on the market will definitely purchase tyres for my other vehicles from here! :)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fodi in Leyton branch best man</t>
+          <t>Happy customer :)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>The Garage Door Centre</t>
+          <t>Garolla</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Very pleased with the Horman roller garage door fitted today. Very professional service from the Garage Door Centre and happy to recommend. Big thank you to Scot and Justin for the fitting today.</t>
+          <t>The team that was sent where fantastic on time no mess explained how the door worked before they left house. Professional job all round.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>The team that was sent where fantastic</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>I was very pleased with the quality of the Hormann Georgian door for the price given. The two guys who fitted it turned up on time were friendly and professional and explained afterwards how to operate and look after the door. My old dented rusting door was removed as well at no extra cost. Compared to some local fitters' prices I was very satisfied. Payment is required in advance; a fifty percent deposit and then the balance 3 days before fitting. This is to stop those despicable people out there who have work done and then do not pay afterwards. I was happy to pay this way and I would highly recommend this company.</t>
+          <t>Very good work well pleased.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Very pleased with my new garage door</t>
+          <t>Roller doors</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Very pleased with my new Hormann sectional garage door from The Garage Door Centre and the whole process from showroom to fitting was straightforward. The installation was completed on schedule and their team were well organised and courteous. I would recommend them.</t>
+          <t>Delighted with Garolla Electric Roller Garage Door.  Installed on the day advised at original survey and left in a tidy and clean state following installation</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Very pleased with the Horman roller…</t>
+          <t>Delighted with Garolla Electric Roller…</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>IN'n'OUT Autocentres</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Forget about it. YOu call and can never get a person; they shunt you to the website which is equally useless.  This was to see about fixing our microwave. They clearly do not want to help you.</t>
+          <t>MOT and interim service - passed the MOT with no issues but they asked for £100 for air filter and £100 for fuel filter ( I thought filters were part of the service) they also said I need a new battery £200 - I sourced exact same battery for £97 air filter (Bosch) £18 - and just ordered fuel filter £18 and will fit them myself saving almost £270</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>MOT and interim service</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>We had ongoing problems since the washer was 6 months old. GE refused to acknowledge despite2-3 service calls because it wouldn't spin or drain properly. The washer's belt and sensor also broke at 2 1/2 years requiring service again. 1 month after our 3year warrant expired through Best Buy it stopped working completely starting with a non spin or drain again. Neither GE or Best Buy extended warranty would cover. GE customer service reps were rude and just do not care that a 3year old washer broke completely. I took this concern to the head supervisor in which she only offered to pay 50% of parts. Absolutely ridiculous. This washer was a complete lemon from the start and GE refused to acknowledge this or the real problem. My husband and I will tell everyone about this experience and never buy a GE product again!</t>
+          <t>Took our Skoda Yeti on 21st February to have 2 new front brake discs and pads fitted. Charged a good price and it was ready to collect 20 minutes before stated.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Do not buy the top…</t>
+          <t>More like In'n'Wait'n'Wait'n'Wait</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Do not buy the top loader-GTW465ASNWWSKU:6325628 GE</t>
+          <t>Excellent. Excellent. Excellent! The Newark on Trent centre never fails to impress with their efficiency professionalism customer care and prices.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Forget about it</t>
+          <t>Excellent</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sheds.co.uk</t>
+          <t>Ring</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Great service shed arrived exactly at the right time and was really easy to build. I also ordered some shelves and a Solar PIR light with my order. The light unfortunately was faulty but after emailing the sheds team Jenny was quick to rectify this and sent out a new PIR light replacement straight away.</t>
+          <t>Ring doorbell.lost my wifi and cant connect.tryed everything that there support suggests and now is a paper waight.i am not impressed.left meeages.tried phone contacts that not reconisable when u phone.not a good service</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Ring doorbell.lost my wifi and cant…</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>1.3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>I would strongly recommend NOT using this company. Took money on day of order and then took 7 months to deliver the log cabin. AND THEN even managed to deliver on the wrong date! There were faults in the log cabin with no reasonable solution; and then they refused to communicate with me. Eventually I had to get my money back from Barclaycard Visa (who were excellent). Sheds.co.uk - an appalling company to do business with.</t>
+          <t>I have been waiting for a new door sensor for weeks they keep telling me they will let me know when it has been sent out but they dont send one out.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Very helpful responses to questions…</t>
+          <t>I think ring camera is great for €3 a…</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Very helpful responses to questions asked regarding chosen shed. Thanks Ellis. Joy O</t>
+          <t xml:space="preserve">I bought this system and it has been nothing but problems. I definatly dont recommend it so many faults poor customer service. </t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Great service</t>
+          <t>Still not replaced new faulty doorbell sensor after 2 MONTHS of waiting! Not good enough</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ring</t>
+          <t>Centralautopoint</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Unlike some other brands such as Canary there is no auto switching of modes ie from home to away when leaving the house. Although it does have geofence. There is no night mode either for when your asleep. You have to manually set it to away mode. The system needs to be updated online with other brands.</t>
+          <t>If you are in need of an honest reliable and friendly garage you found it.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>If you are in need of an hones tGarage look no further.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Kept losing the signal when I was setting it up. I was only two yards away from the router so what will it be like when it’s further away and outside? I use my laptop at a much further distance and have no problem with that. The app on the phone and the Fire tablet was very slow to respond sometimes not working at all even when there was a WiFi signal. On the plus side when it was working the picture quality was pretty good but that is only the good thing I can say. Returned mine for a refund.</t>
+          <t>I was not disappointed.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Dont buy these out door camera</t>
+          <t>Really impressed!</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Dont buy these products i bought a outside camera it has intermitting notifications i checked on line to contact the support the online bot gave me a number i called the number it then cost me £30 because this was not a uk number. After 50 minutes on the line they have now told me i need one of their WIFI extenders because the signal is week. I was told it could be a wall blocking the signal the camera is a outdoor one so there will be a wall. I would buy another make of camera these are terrible.</t>
+          <t>Booked my car in for the second year for a major service and MOT this time.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Unlike some other brands such as Canary…</t>
+          <t>Not what I asked for</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>National Tyres and Autocare</t>
+          <t>E.ON SE</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>I buy new tyres from National Tyres in Portsmouth and they fixed wrong inside place to outside ridiculous</t>
+          <t>The wait on phone is really bad 1 half hours disgraceful.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>The wait on phone is really bad 1 half…</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">As always Top quality Service from National Tyres and Autocare at 317 Purley Way. </t>
+          <t>Looks like the only was is to cancel my direct debit to get them to contact me they will try and charge me for it but I've done everything possible so good luck with that.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Recent Purchase</t>
+          <t>Trying to find a non existant electric…</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>The site was very slow to load and I found the different tyre options a bit confusing.  Unable to find out if bluelight discount can be applied.</t>
+          <t>Can't get hold of eon customer service phoned them and was on hold for an hour with no answer went on the online chat and was told to phone them tried to send them an email and it was returned went on FB messenger and was told to wait.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>They is irresponsible</t>
+          <t>Can't get hold of eon customer service</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Rated People</t>
+          <t>Mr Clutch</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Very simple to use. Quite happy.</t>
+          <t>Fodi in Leyton branch best man very helpfulservice was great highly recommend !</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Fodi in Leyton branch best man</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>Warning! We’ve detected misuse on this page</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Very happy with your website and will use it whenever I need a job doing.</t>
+          <t xml:space="preserve">I booked my car in at the Chelmsford branch and Chris was my first contact a delightful man with perfect manners and so helpful I limped my car into the Chelmsford branch and as he promised Chris and his team had my car running perfectly by mid day I am very satisfied and will be using them for any job that comes up in the future. </t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Easy to usestraightforward</t>
+          <t>I booked my car in at the Chelmsford…</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Easy to usestraightforward job explained and your site went to work found me several companies. The one I used was quick and efficient in replying to my requestand also completing the job .</t>
+          <t>Excellent service from the manager Steve I really cannot recommend them enough. Got my MOT done at the Chingford branch! Well done guys i appreciate it!</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Very simple to use</t>
+          <t>Excellent service from the manager…</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Facebook</t>
+          <t>The Garage Door Centre</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>So I joined facebook about 2 months ago and literally the only thing I did was join my town's community page. I didn't post anything I didn't add anyone I didn't write any comments and in fact I haven't even gone on the platform in quite some time. Despite all this my account has been disabled FOUR TIMES for supposedly "violating the community standards". And somehow I've been on instagram for nearly a year and NEVER ONCE had this problem. Honestly as soon as it gets re-enabled again I'm just deleting my account because I'm sick of dealing with this</t>
+          <t>Very pleased with the Horman roller garage door fitted today. Very professional service from the Garage Door Centre and happy to recommend. Big thank you to Scot and Justin for the fitting today.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Very pleased with the Horman roller…</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.2</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>THANK YOU VERY VERY MUCH FOR BEING IMPECCABLY FLAWLESS AND IMMACULATE TO THE VERY HIGHEST DEGREE!</t>
+          <t>I was very pleased with the quality of the Hormann Georgian door for the price given. The two guys who fitted it turned up on time were friendly and professional and explained afterwards how to operate and look after the door. My old dented rusting door was removed as well at no extra cost. Compared to some local fitters' prices I was very satisfied. Payment is required in advance; a fifty percent deposit and then the balance 3 days before fitting. This is to stop those despicable people out there who have work done and then do not pay afterwards. I was happy to pay this way and I would highly recommend this company.</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Worst service I've ever gotten from a website</t>
+          <t>Quality and value and professional</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ABSOLUTE PERFECTION GUARANTEED! It successfully taught me the importance of responsible communication! I became a lot more diplomatic tactful courteous and respectful! </t>
+          <t>Very pleased with my new Hormann sectional garage door from The Garage Door Centre and the whole process from showroom to fitting was straightforward. The installation was completed on schedule and their team were well organised and courteous. I would recommend them.</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>artificial picture of lives</t>
+          <t>Very pleased with my new garage door</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>etyres</t>
+          <t>GE</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Great service ordered my tyres paid extra for mobile tyre fitter. Tyres came with fitter and the guy fitted them within 20 minutes.</t>
+          <t>Forget about it. YOu call and can never get a person; they shunt you to the website which is equally useless.  This was to see about fixing our microwave. They clearly do not want to help you.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Forget about it</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Abysmal!!!</t>
+          <t>We had ongoing problems since the washer was 6 months old. GE refused to acknowledge despite2-3 service calls because it wouldn't spin or drain properly. The washer's belt and sensor also broke at 2 1/2 years requiring service again. 1 month after our 3year warrant expired through Best Buy it stopped working completely starting with a non spin or drain again. Neither GE or Best Buy extended warranty would cover. GE customer service reps were rude and just do not care that a 3year old washer broke completely. I took this concern to the head supervisor in which she only offered to pay 50% of parts. Absolutely ridiculous. This washer was a complete lemon from the start and GE refused to acknowledge this or the real problem. My husband and I will tell everyone about this experience and never buy a GE product again!</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Happy customer :)</t>
+          <t>Awful Customer Service</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Brilliant easy to navigate website and cheapest tyres on the market will definitely purchase tyres for my other vehicles from here! :)</t>
+          <t>Do not buy the top loader-GTW465ASNWWSKU:6325628 GE</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Fantastic tyre service</t>
+          <t>Do not buy the top…</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Garolla</t>
+          <t>Sheds.co.uk</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>The team that was sent where fantastic on time no mess explained how the door worked before they left house. Professional job all round.</t>
+          <t>Great service shed arrived exactly at the right time and was really easy to build. I also ordered some shelves and a Solar PIR light with my order. The light unfortunately was faulty but after emailing the sheds team Jenny was quick to rectify this and sent out a new PIR light replacement straight away.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Great service</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Very good work well pleased.</t>
+          <t>I would strongly recommend NOT using this company. Took money on day of order and then took 7 months to deliver the log cabin. AND THEN even managed to deliver on the wrong date! There were faults in the log cabin with no reasonable solution; and then they refused to communicate with me. Eventually I had to get my money back from Barclaycard Visa (who were excellent). Sheds.co.uk - an appalling company to do business with.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Delighted with Garolla Electric Roller…</t>
+          <t>WARNING - DO NOT USE THIS COMPANY</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Delighted with Garolla Electric Roller Garage Door.  Installed on the day advised at original survey and left in a tidy and clean state following installation</t>
+          <t>Very helpful responses to questions asked regarding chosen shed. Thanks Ellis. Joy O</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>The team that was sent where fantastic</t>
+          <t>Very helpful responses to questions…</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IN'n'OUT Autocentres</t>
+          <t>Ring</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>MOT and interim service - passed the MOT with no issues but they asked for £100 for air filter and £100 for fuel filter ( I thought filters were part of the service) they also said I need a new battery £200 - I sourced exact same battery for £97 air filter (Bosch) £18 - and just ordered fuel filter £18 and will fit them myself saving almost £270</t>
+          <t>Unlike some other brands such as Canary there is no auto switching of modes ie from home to away when leaving the house. Although it does have geofence. There is no night mode either for when your asleep. You have to manually set it to away mode. The system needs to be updated online with other brands.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Unlike some other brands such as Canary…</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>1.6</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Took our Skoda Yeti on 21st February to have 2 new front brake discs and pads fitted. Charged a good price and it was ready to collect 20 minutes before stated.</t>
+          <t>Kept losing the signal when I was setting it up. I was only two yards away from the router so what will it be like when it’s further away and outside? I use my laptop at a much further distance and have no problem with that. The app on the phone and the Fire tablet was very slow to respond sometimes not working at all even when there was a WiFi signal. On the plus side when it was working the picture quality was pretty good but that is only the good thing I can say. Returned mine for a refund.</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Excellent</t>
+          <t>Ring Video Doorbell</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Excellent. Excellent. Excellent! The Newark on Trent centre never fails to impress with their efficiency professionalism customer care and prices.</t>
+          <t>Dont buy these products i bought a outside camera it has intermitting notifications i checked on line to contact the support the online bot gave me a number i called the number it then cost me £30 because this was not a uk number. After 50 minutes on the line they have now told me i need one of their WIFI extenders because the signal is week. I was told it could be a wall blocking the signal the camera is a outdoor one so there will be a wall. I would buy another make of camera these are terrible.</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>MOT and interim service</t>
+          <t>Dont buy these out door camera</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ring</t>
+          <t>National Tyres and Autocare</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Ring doorbell.lost my wifi and cant connect.tryed everything that there support suggests and now is a paper waight.i am not impressed.left meeages.tried phone contacts that not reconisable when u phone.not a good service</t>
+          <t>I buy new tyres from National Tyres in Portsmouth and they fixed wrong inside place to outside ridiculous</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>simple and effective</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>I have been waiting for a new door sensor for weeks they keep telling me they will let me know when it has been sent out but they dont send one out.</t>
+          <t xml:space="preserve">As always Top quality Service from National Tyres and Autocare at 317 Purley Way. </t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Still not replaced new faulty doorbell sensor after 2 MONTHS of waiting! Not good enough</t>
+          <t>Recent Purchase</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t xml:space="preserve">I bought this system and it has been nothing but problems. I definatly dont recommend it so many faults poor customer service. </t>
+          <t>The site was very slow to load and I found the different tyre options a bit confusing.  Unable to find out if bluelight discount can be applied.</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Ring doorbell.lost my wifi and cant…</t>
+          <t>They is irresponsible</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Rated People</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>my favorite website they are proven to pay me now I just work at home in this time of pandemic now they really pay thank you</t>
+          <t xml:space="preserve">Very disappointed </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Write a review</t>
+          <t>Very disappointed</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Outstanding application to feel free from threats. Enjoy to use twitter more than before with this friendly app...</t>
+          <t>Very simple to use. Quite happy.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Very good service for the affordable…</t>
+          <t>Easy to usestraightforward</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Very good service for the affordable price! Their IPTV activation is very fast and customer support also best. It’s the best streaming service with full HD quality. My experience is great on bestiptvfrance. Highly recommended service!!!</t>
+          <t>for people who buy these leads  do not waste your time and money because if you are not membership you do not receive any help even if you pay for the lead 2 minutes after receiving the customer's number he has changed his mind and does not want to do this job it is disgusting that Rated  People.  I do not return money for such cases I do not recommend it</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>AMAZING</t>
+          <t>Very simple to use</t>
         </is>
       </c>
     </row>

</xml_diff>